<commit_message>
Ajout des questions du Quizz dans la feuille 2
</commit_message>
<xml_diff>
--- a/POLITICUS questions.xlsx
+++ b/POLITICUS questions.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
   <si>
     <t>INTITULE QUESTION</t>
   </si>
@@ -170,6 +171,261 @@
   </si>
   <si>
     <t>SOMME</t>
+  </si>
+  <si>
+    <t>RESULTAT</t>
+  </si>
+  <si>
+    <t>571 députés et 338 sénateurs</t>
+  </si>
+  <si>
+    <t>Le Parlement français est composé de deux chambres, l'Assemblée nationale et le Sénat qui ont respectivement, jusqu'en 2010</t>
+  </si>
+  <si>
+    <t>REPONSE</t>
+  </si>
+  <si>
+    <t>577 députés et 343 sénateurs</t>
+  </si>
+  <si>
+    <t>574 députés et 335 sénateurs</t>
+  </si>
+  <si>
+    <t>581 députés et 348 sénateurs</t>
+  </si>
+  <si>
+    <t>Les deux chambres du Parlement siègent respectivement</t>
+  </si>
+  <si>
+    <t>Au Palais Bourbon pour les députés, au Palais du Luxembourg pour les sénateurs</t>
+  </si>
+  <si>
+    <t>Au Palais du Luxembourg pour les députés, au Palais Bourbon pour les sénateurs</t>
+  </si>
+  <si>
+    <t>Au Palais Royal pour les députés, au Palais du Luxembourg pour les sénateurs</t>
+  </si>
+  <si>
+    <t>Au Grand Palais pour les députés, au Palais Royal pour les sénateurs</t>
+  </si>
+  <si>
+    <t>Le Parlement se réunit en une session ordinaire</t>
+  </si>
+  <si>
+    <t>De 9 mois</t>
+  </si>
+  <si>
+    <t>Permanente</t>
+  </si>
+  <si>
+    <t>De 8 mois</t>
+  </si>
+  <si>
+    <t>De 10 mois</t>
+  </si>
+  <si>
+    <t>Le Parlement exerce le pouvoir</t>
+  </si>
+  <si>
+    <t>Législatif</t>
+  </si>
+  <si>
+    <t>Réglementaire</t>
+  </si>
+  <si>
+    <t>Administratif</t>
+  </si>
+  <si>
+    <t>Absolu</t>
+  </si>
+  <si>
+    <t>L'initiative des lois appartient, selon la Constitution,</t>
+  </si>
+  <si>
+    <t>Concurremment au Premier ministre et aux membres du Parlement</t>
+  </si>
+  <si>
+    <t>Aux seuls membres du Parlement</t>
+  </si>
+  <si>
+    <t>Concurremment au Président de la République, au Premier ministre et aux membres du Parlement</t>
+  </si>
+  <si>
+    <t>Concurremment aux différents ministres et aux membres du Parlement</t>
+  </si>
+  <si>
+    <t>Depuis 1995, l'ordre du jour est arrêté par chaque Assemblée à l'initiative des groupes d'opposition ainsi qu'à celle des groupes minoritaires</t>
+  </si>
+  <si>
+    <t>Un jour de séance par mois</t>
+  </si>
+  <si>
+    <t>Trois jours de séance par mois</t>
+  </si>
+  <si>
+    <t>Huit jours de séance par mois</t>
+  </si>
+  <si>
+    <t>Dix jours de séance par mois</t>
+  </si>
+  <si>
+    <t>Le mouvement d'un texte en discussion entre les députés et les sénateurs pour faire voter une loi s'appelle</t>
+  </si>
+  <si>
+    <t>La navette parlementaire</t>
+  </si>
+  <si>
+    <t>Le cavalier législatif</t>
+  </si>
+  <si>
+    <t>La commission mixte paritaire parlementaire</t>
+  </si>
+  <si>
+    <t>Le va-et-vient parlementaire</t>
+  </si>
+  <si>
+    <t>Il y a 577 députés et 348 sénateurs qui seront prévus dêtre élus en 2011</t>
+  </si>
+  <si>
+    <t>Il y a 572 députés et 339 sénateurs qui seront prévus dêtre élus en 2011</t>
+  </si>
+  <si>
+    <t>Il y a 583 députés et 351 sénateurs qui seront prévus dêtre élus en 2011</t>
+  </si>
+  <si>
+    <t>Il y a 576 députés et 337 sénateurs qui seront prévus dêtre élus en 2011</t>
+  </si>
+  <si>
+    <t>Le mode d'élection des parlementaires est le scrutin uninominal à 2 tours pour les députés, le scrutin universel indirect pour les sénateurs</t>
+  </si>
+  <si>
+    <t>Le mode d'élection des parlementaires est le scrutin proportionnel plurinominal à 2 tours pour les députés, le scrutin universel direct pour les sénateurs</t>
+  </si>
+  <si>
+    <t>Le mode d'élection des parlementaires est le scrutin direct uninominal à 2 tours pour les députés, le scrutin universel indirect pour les sénateurs</t>
+  </si>
+  <si>
+    <t>Il faut avoir au moins 18 ans pour être député et au moins 24 ans pour être sénateur</t>
+  </si>
+  <si>
+    <t>Le mode d'élection des parlementaires est le scrutin majoritaire plurinominal à 2 tours pour les députés, le scrutin universel direct pour les sénateurs</t>
+  </si>
+  <si>
+    <t>Il faut avoir au moins 21 ans pour être député et au moins 28 ans pour être sénateur</t>
+  </si>
+  <si>
+    <t>Il faut avoir au moins 25 ans pour être député et au moins 32 ans pour être sénateur</t>
+  </si>
+  <si>
+    <t>Il faut avoir au moins 25 ans pour être député et au moins 35 ans pour être sénateur</t>
+  </si>
+  <si>
+    <t>Une inviolabilité pénale totale ne fait pas partie du statut du parlementaire</t>
+  </si>
+  <si>
+    <t>Une indemnité ne fait pas partie du statut du parlementaire</t>
+  </si>
+  <si>
+    <t>Une irresponsabilité parlementaire quant à ses opinions et son vote dans le cadre de son travail parlementaire ne fait pas partie du statut du parlementaire</t>
+  </si>
+  <si>
+    <t>Des incompatibilités de fonction ne fait pas partie du statut du parlementaire</t>
+  </si>
+  <si>
+    <t>La session ordinaire est ouverte et fermée par décret du Premier ministre</t>
+  </si>
+  <si>
+    <t>La session ordinaire est ouverte et fermée par décret du Président de la République</t>
+  </si>
+  <si>
+    <t>La session ordinaire est ouverte et fermée par arrêté conjoint des présidents des deux Assemblées</t>
+  </si>
+  <si>
+    <t>Il n'y a pas d'acte, c'est la Constitution qui fixe la période d'ouverture et de fermeture de la session ordinaire</t>
+  </si>
+  <si>
+    <t>Les sessions extraordinaires s'ouvrent et se ferment par décret du Président de la République</t>
+  </si>
+  <si>
+    <t>Les sessions extraordinaires s'ouvrent et se ferment par décret du Premier ministre</t>
+  </si>
+  <si>
+    <t>Les sessions extraordinaires s'ouvrent et se ferment par arrêté conjoint des présidents des deux Assemblées</t>
+  </si>
+  <si>
+    <t>Il n'y a pas d'acte, c'est la Constitution qui fixe la période d'ouverture et de fermeture des sessions extraordinaires</t>
+  </si>
+  <si>
+    <t>On peut trouver le compte rendu intégral des débats du Parlement selon la Constitution au Journal Officiel de la République française</t>
+  </si>
+  <si>
+    <t>On peut trouver le compte rendu intégral des débats du Parlement selon la Constitution sur le site internet de chacune des deux Assemblées (depuis 2003)</t>
+  </si>
+  <si>
+    <t>On peut trouver le compte rendu intégral des débats du Parlement selon la Constitution à la fois sur le site internet de chacune des deux Assemblées (depuis 2003) et au Journal Officiel de la République française</t>
+  </si>
+  <si>
+    <t>On peut trouver le compte rendu intégral des débats du Parlement selon la Constitution dans un numéro spécial de chaque ministère et qui paraît tous les 15 jours</t>
+  </si>
+  <si>
+    <t>La Constitution cite les domaines où la loi fixe les règles et ceux dont elle détermine les principes fondamentaux. La préservation de l'environnement relève des principes fondamentaux</t>
+  </si>
+  <si>
+    <t>La Constitution cite les domaines où la loi fixe les règles et ceux dont elle détermine les principes fondamentaux. La création de catégories d'établissements publics relève des principes fondamentaux</t>
+  </si>
+  <si>
+    <t>La Constitution cite les domaines où la loi fixe les règles et ceux dont elle détermine les principes fondamentaux. La nationalité, l'état et la capacité des personnes, les régimes matrimoniaux, les successions et libéralités relève des principes fondamentaux</t>
+  </si>
+  <si>
+    <t>La Constitution cite les domaines où la loi fixe les règles et ceux dont elle détermine les principes fondamentaux. L'assiette, le taux et les modalités de recouvrement des impositions de toutes natures ; le régime d'émission de la monnaie relève des principes fondamentaux</t>
+  </si>
+  <si>
+    <t>C'est Alain Poher qui assuma en 1969 et 1974 l'intérim de la Présidence de la République</t>
+  </si>
+  <si>
+    <t>C'est Gaston Monnerville qui assuma en 1969 et 1974 l'intérim de la Présidence de la République</t>
+  </si>
+  <si>
+    <t>C'est René Monory qui assuma en 1969 et 1974 l'intérim de la Présidence de la République</t>
+  </si>
+  <si>
+    <t>C'est Christian Poncelet qui assuma en 1969 et 1974 l'intérim de la Présidence de la République</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Elles n'ont pas un caractère législatif dès leur publication". C'est une caractéristique des ordonnances que le Gouvernement peut prendre sur autorisation du Parlement dans un domaine qui est normalement du domaine de la loi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Elles sont prises en Conseil des Ministres après avis du Conseil d'État". C'est une caractéristique des ordonnances que le Gouvernement peut prendre sur autorisation du Parlement dans un domaine qui est normalement du domaine de la loi </t>
+  </si>
+  <si>
+    <t>"Elles entrent en vigueur dès leur publication mais deviennent caduques si le projet de loi de ratification n'est pas déposé devant le Parlement". C'est une caractéristique des ordonnances que le Gouvernement peut prendre sur autorisation du Parlement dans un domaine qui est normalement du domaine de la loi .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Elles ne peuvent être ratifiées que de manière expresse". C'est une caractéristique des ordonnances que le Gouvernement peut prendre sur autorisation du Parlement dans un domaine qui est normalement du domaine de la loi </t>
+  </si>
+  <si>
+    <t>Relatif à la motion de censure, elle n'intervient que si le Président de l'Assemblée nationale donne son accord à son dépôt</t>
+  </si>
+  <si>
+    <t>Relatif à la motion de censure, elle est signée par un dixième au moins des membres de l'Assemblée nationale</t>
+  </si>
+  <si>
+    <t>Relatif à la motion de censure, le vote ne peut avoir lieu que quarante-huit heures après son dépôt</t>
+  </si>
+  <si>
+    <t>Relatif à la motion de censure, une majorité de votes favorables oblige le Premier ministre à remettre au Président de la République la démission du Gouvernement</t>
+  </si>
+  <si>
+    <t>Le parlement dispose de 70 jours pour voter la loi de finances (le budget) de l'année suivante</t>
+  </si>
+  <si>
+    <t>Le parlement dispose de 50 jours pour voter la loi de finances (le budget) de l'année suivante</t>
+  </si>
+  <si>
+    <t>Le parlement dispose de 60 jours pour voter la loi de finances (le budget) de l'année suivante</t>
+  </si>
+  <si>
+    <t>Le parlement dispose de 80 jours pour voter la loi de finances (le budget) de l'année suivante</t>
   </si>
 </sst>
 </file>
@@ -492,9 +748,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,4 +1244,664 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>122</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>123</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>125</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>126</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mise à jour des questions du Quizz dans la feuille3
</commit_message>
<xml_diff>
--- a/POLITICUS questions.xlsx
+++ b/POLITICUS questions.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elhy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elhy/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="183">
   <si>
     <t>INTITULE QUESTION</t>
   </si>
@@ -426,6 +427,174 @@
   </si>
   <si>
     <t>Le parlement dispose de 80 jours pour voter la loi de finances (le budget) de l'année suivante</t>
+  </si>
+  <si>
+    <t>Les 577 députés français siègent à l'Assemblée nationale.</t>
+  </si>
+  <si>
+    <t>Les 577 députés français siègent au Sénat.</t>
+  </si>
+  <si>
+    <t>C'est le président de la République qui nomme le Premier ministre.</t>
+  </si>
+  <si>
+    <t>François Mitterand a été président pendant 14 ans.</t>
+  </si>
+  <si>
+    <t>François Mitterand a été président pendant 10 ans.</t>
+  </si>
+  <si>
+    <t>Le principal parti centriste s'appelle LE MODEM.</t>
+  </si>
+  <si>
+    <t>Nicolas Sarkozy appartient au parti de l'UMP.</t>
+  </si>
+  <si>
+    <t>Nicolas Sarkozy appartient au parti du RPR.</t>
+  </si>
+  <si>
+    <t>Ségolène Royal appartient au PS. PS signifie Parti Socialiste.</t>
+  </si>
+  <si>
+    <t>Ségolène Royal appartient au PS. PS signifie Peuple Souverain.</t>
+  </si>
+  <si>
+    <t>Depuis 2000, le président de la République est élu pour 5 ans.</t>
+  </si>
+  <si>
+    <t>Depuis 2000, le président de la République est élu pour 7 ans.</t>
+  </si>
+  <si>
+    <t>Le nom du principal parti écologiste en France est les Verts.</t>
+  </si>
+  <si>
+    <t>Le premier parti politique du premier président français de la Vème République est le RPF.</t>
+  </si>
+  <si>
+    <t>Dans le sigle PCF, le C signifie Communiste.</t>
+  </si>
+  <si>
+    <t>Dans le sigle PCF, le C signifie Capitaliste.</t>
+  </si>
+  <si>
+    <t>C'est le Conseil constitutionnel qui nomme le Premier ministre.</t>
+  </si>
+  <si>
+    <t>Le principal parti centriste s'appelle l'UMP.</t>
+  </si>
+  <si>
+    <t>Le nom du principal parti écologiste en France est les Protecteurs.</t>
+  </si>
+  <si>
+    <t>Le premier parti politique du premier président français de la Vème République est l'UDR.</t>
+  </si>
+  <si>
+    <t>La IV eme république a été instituée en 1947.</t>
+  </si>
+  <si>
+    <t>La IV eme république a été instituée en 1927.</t>
+  </si>
+  <si>
+    <t>En 2007, sous le gouvernement Fillon, une nouvelle fonction est apparue, il s’agit de celle de : Haut-commissaire</t>
+  </si>
+  <si>
+    <t>En 2007, sous le gouvernement Fillon, une nouvelle fonction est apparue, il s’agit de celle de : Ministre adjoint</t>
+  </si>
+  <si>
+    <t>Une proposition de loi ne peut être présentée que par : Un groupe de députés et de sénateurs.</t>
+  </si>
+  <si>
+    <t>Une proposition de loi ne peut être présentée que par : Le parlement.</t>
+  </si>
+  <si>
+    <t>Les trois couleurs, bleu-blanc-rouge, du drapeau français ont pour origine : Le blanc de la royauté et le bleu et rouge de la ville de Paris.</t>
+  </si>
+  <si>
+    <t>Les trois couleurs, bleu-blanc-rouge, du drapeau français ont pour origine : Le blanc de la pureté, le bleu du ciel et le rouge du sang  de la Révolution.</t>
+  </si>
+  <si>
+    <t>L'année parlementaire débute le 1er octobre.</t>
+  </si>
+  <si>
+    <t>Symbole de la République, Marianne est : Le nom d'une sainte qui s'est sacrifiée au nom de la liberté.</t>
+  </si>
+  <si>
+    <t>Symbole de la République, Marianne est : La contraction de deux prénoms largement répandus chez les reines à l'époque de la Révolution.</t>
+  </si>
+  <si>
+    <t>L'année parlementaire débute le 1er mai.</t>
+  </si>
+  <si>
+    <t>Les députés siègent: Au Palais-Bourbon</t>
+  </si>
+  <si>
+    <t>Les députés siègent: Au Palais-Bourdon</t>
+  </si>
+  <si>
+    <t>Le premier président de la République fut: Louis Napoléon Bonaparte.</t>
+  </si>
+  <si>
+    <t>Le premier président de la République fut: Jules César.</t>
+  </si>
+  <si>
+    <t>Quel président a fait rédiger la Constitution de la Ve République : Le général de Gaulle.</t>
+  </si>
+  <si>
+    <t>Quel président a fait rédiger la Constitution de la Ve République : Giscard d'Estaing.</t>
+  </si>
+  <si>
+    <t>Le bonnet phrygien, symbole de la République, était porté à l’origine par : Les esclaves affranchis de l'Empire romain.</t>
+  </si>
+  <si>
+    <t>Le bonnet phrygien, symbole de la République, était porté à l’origine par : La femme de Socrate.</t>
+  </si>
+  <si>
+    <t>Une session parlementaire dure : Neuf mois.</t>
+  </si>
+  <si>
+    <t>Une session parlementaire dure : Trois mois.</t>
+  </si>
+  <si>
+    <t>La Phrygie était : Un royaume d'Asie mineure.</t>
+  </si>
+  <si>
+    <t>La Phrygie était : Une prêtresse émettant des oracles.</t>
+  </si>
+  <si>
+    <t>Les femmes ont obtenu le droit de vote en France en : 1944</t>
+  </si>
+  <si>
+    <t>Les femmes ont obtenu le droit de vote en France en : 1954</t>
+  </si>
+  <si>
+    <t>Quand on parle du Quai d’Orsay, on fait référence au ministère : Des Affaires étrangères.</t>
+  </si>
+  <si>
+    <t>Quand on parle du Quai d’Orsay, on fait référence au ministère : De l'Economie.</t>
+  </si>
+  <si>
+    <t>Repris d’un poème d’Arthur Rimbaud, un mot de Jacques Chirac a fait une entrée fracassante en politique en 2000, il s’agit de : Abracadabrantesque.</t>
+  </si>
+  <si>
+    <t>Repris d’un poème d’Arthur Rimbaud, un mot de Jacques Chirac a fait une entrée fracassante en politique en 2000, il s’agit de : Chienlit</t>
+  </si>
+  <si>
+    <t>Jusqu’en 1848, les élections ne se font pas au suffrage universel mais au suffrage censitaire, cela signifie que seuls votent : Ceux qui paient un certain montant d'impôt.</t>
+  </si>
+  <si>
+    <t>Jusqu’en 1848, les élections ne se font pas au suffrage universel mais au suffrage censitaire, cela signifie que seuls votent : Les nobles.</t>
+  </si>
+  <si>
+    <t>Qui a dit : « Moi, les hommes politiques, j’appelle ça des timbres. De face, ils vous sourient, ils sont figés. Mais si jamais vous leur passez la main dans le dos, alors là, ça colle ! ». C'est Coluche.</t>
+  </si>
+  <si>
+    <t>Qui a dit : « Moi, les hommes politiques, j’appelle ça des timbres. De face, ils vous sourient, ils sont figés. Mais si jamais vous leur passez la main dans le dos, alors là, ça colle ! ». C'est Jean-Marie Bigard.</t>
+  </si>
+  <si>
+    <t>La première femme candidate à l’élection présidentielle en France a été : Arlette Laguillier.</t>
+  </si>
+  <si>
+    <t>La première femme candidate à l’élection présidentielle en France a été : Elisabeth DUONG.</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
@@ -1904,4 +2073,470 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="164.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>174</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>177</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>178</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>179</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>182</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>